<commit_message>
running analysis with new gRNAs
</commit_message>
<xml_diff>
--- a/data/gRNAList.xlsx
+++ b/data/gRNAList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="384">
   <si>
     <t xml:space="preserve">Citation</t>
   </si>
@@ -1091,6 +1091,87 @@
   </si>
   <si>
     <t xml:space="preserve">CTT.TTAGAAAACAAAATCCAGAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gRNA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TTAGACCAGATCTGAGCCT.NGG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCN.GACTGTACTGGGTCTCTCTG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gLTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gnef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTGGCTAGAAGCACAAGAGG.NGG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gtat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCCACCTCCCAACCCCGAG.NGG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gpol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAGTACAATGTGCTTCCACA.NGG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTTACACCCTATGAGCCAGCA.NGG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GagB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCCTTCCCACAAGGGAAGGCCA.NGG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GagC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCGAGAGCGTCGGTATTAAGCG.NGG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GagD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GGATAGATGTAAAAGACACCA.NGG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PolB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dCas9 NF-kB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTACAAGGGACTTTCCGCTG.NGG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dCas9 Sp1-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCATGGGCGGGACCGGGGAG.NGG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dCas9 Sp1-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCGTGGCATGGGCGGGACCG.NGG</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1129,6 +1210,34 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9.3"/>
+      <color rgb="FF575757"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="AdvOT1ef757c0"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1181,13 +1290,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1199,6 +1324,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF575757"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1207,21 +1392,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F211"/>
+  <dimension ref="A1:F230"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="I226" activeCellId="0" sqref="I226"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.8825910931174"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +1425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>23974631</v>
       </c>
@@ -1261,7 +1445,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>23974631</v>
       </c>
@@ -1281,7 +1465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>25049410</v>
       </c>
@@ -1301,7 +1485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>25049410</v>
       </c>
@@ -1321,7 +1505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>25049410</v>
       </c>
@@ -1341,7 +1525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>25049410</v>
       </c>
@@ -1361,7 +1545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1381,7 +1565,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1401,7 +1585,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1421,7 +1605,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1441,7 +1625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1461,7 +1645,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1481,7 +1665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1501,7 +1685,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1521,7 +1705,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1541,7 +1725,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1561,7 +1745,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1581,7 +1765,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1601,7 +1785,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1621,7 +1805,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1641,7 +1825,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1661,7 +1845,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1681,7 +1865,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1701,7 +1885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1721,7 +1905,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1741,7 +1925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1761,7 +1945,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1781,7 +1965,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>25752527</v>
       </c>
@@ -1801,7 +1985,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>25808449</v>
       </c>
@@ -1821,7 +2005,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>25808449</v>
       </c>
@@ -1841,7 +2025,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>25808449</v>
       </c>
@@ -1861,7 +2045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>25808449</v>
       </c>
@@ -1881,7 +2065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>25808449</v>
       </c>
@@ -1901,7 +2085,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>25808449</v>
       </c>
@@ -1921,7 +2105,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>25808449</v>
       </c>
@@ -1941,7 +2125,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>25808449</v>
       </c>
@@ -1961,7 +2145,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>25808449</v>
       </c>
@@ -1981,7 +2165,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>25808449</v>
       </c>
@@ -2001,7 +2185,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2021,7 +2205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2041,7 +2225,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2061,7 +2245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2081,7 +2265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2101,7 +2285,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2121,7 +2305,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2141,7 +2325,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2161,7 +2345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2181,7 +2365,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2201,7 +2385,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2221,7 +2405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2241,7 +2425,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2261,7 +2445,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2281,7 +2465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2301,7 +2485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>26538064</v>
       </c>
@@ -2321,7 +2505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2341,7 +2525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2361,7 +2545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2381,7 +2565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2401,7 +2585,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2421,7 +2605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2441,7 +2625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2461,7 +2645,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2481,7 +2665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2501,7 +2685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2521,7 +2705,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2541,7 +2725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2561,7 +2745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2581,7 +2765,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2601,7 +2785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2621,7 +2805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2641,7 +2825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2661,7 +2845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2681,7 +2865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2701,7 +2885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2721,7 +2905,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2741,7 +2925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2761,7 +2945,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2781,7 +2965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2801,7 +2985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2821,7 +3005,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2841,7 +3025,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>26581162</v>
       </c>
@@ -2861,7 +3045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>26607397</v>
       </c>
@@ -2881,7 +3065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>26607397</v>
       </c>
@@ -2901,7 +3085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
         <v>26607397</v>
       </c>
@@ -2921,7 +3105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
         <v>26607397</v>
       </c>
@@ -2941,7 +3125,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
         <v>26607397</v>
       </c>
@@ -2961,7 +3145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
         <v>26607397</v>
       </c>
@@ -2981,7 +3165,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
         <v>26607397</v>
       </c>
@@ -3001,7 +3185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
         <v>26775808</v>
       </c>
@@ -3021,7 +3205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <v>26775808</v>
       </c>
@@ -3041,7 +3225,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
         <v>26775808</v>
       </c>
@@ -3061,7 +3245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
         <v>26775808</v>
       </c>
@@ -3081,7 +3265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
         <v>26775808</v>
       </c>
@@ -3101,7 +3285,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
         <v>26775808</v>
       </c>
@@ -3121,7 +3305,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
         <v>26775808</v>
       </c>
@@ -3141,7 +3325,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
         <v>26775808</v>
       </c>
@@ -3161,7 +3345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
         <v>26775808</v>
       </c>
@@ -3181,7 +3365,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
         <v>26775808</v>
       </c>
@@ -3201,7 +3385,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
         <v>26775808</v>
       </c>
@@ -3221,7 +3405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="n">
         <v>26775808</v>
       </c>
@@ -3241,7 +3425,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3261,7 +3445,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3281,7 +3465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3301,7 +3485,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3321,7 +3505,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3341,7 +3525,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3361,7 +3545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3381,7 +3565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3401,7 +3585,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3421,7 +3605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3441,7 +3625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3461,7 +3645,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3481,7 +3665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3501,7 +3685,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3521,7 +3705,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3541,7 +3725,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3561,7 +3745,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3581,7 +3765,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3601,7 +3785,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="n">
         <v>26796669</v>
       </c>
@@ -3621,7 +3805,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="n">
         <v>26939770</v>
       </c>
@@ -3641,7 +3825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="n">
         <v>26939770</v>
       </c>
@@ -3661,7 +3845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="n">
         <v>26939770</v>
       </c>
@@ -3681,7 +3865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="n">
         <v>26939770</v>
       </c>
@@ -3701,7 +3885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3721,7 +3905,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3741,7 +3925,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3761,7 +3945,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3781,7 +3965,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3801,7 +3985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3821,7 +4005,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3841,7 +4025,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3861,7 +4045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3881,7 +4065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3901,7 +4085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3921,7 +4105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3941,7 +4125,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3961,7 +4145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -3981,7 +4165,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -4001,7 +4185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -4021,7 +4205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -4041,7 +4225,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -4061,7 +4245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -4081,7 +4265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -4101,7 +4285,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -4121,7 +4305,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -4141,7 +4325,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -4161,7 +4345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -4181,7 +4365,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -4201,7 +4385,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="n">
         <v>26990633</v>
       </c>
@@ -4221,7 +4405,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="n">
         <v>27068471</v>
       </c>
@@ -4241,7 +4425,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="n">
         <v>27068471</v>
       </c>
@@ -4261,7 +4445,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="n">
         <v>27068471</v>
       </c>
@@ -4281,7 +4465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="n">
         <v>27068471</v>
       </c>
@@ -4301,7 +4485,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="n">
         <v>27068471</v>
       </c>
@@ -4321,7 +4505,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="n">
         <v>27068471</v>
       </c>
@@ -4341,7 +4525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="n">
         <v>27068471</v>
       </c>
@@ -4361,7 +4545,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="n">
         <v>27068471</v>
       </c>
@@ -4381,7 +4565,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="n">
         <v>27194423</v>
       </c>
@@ -4401,7 +4585,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="n">
         <v>27194423</v>
       </c>
@@ -4421,7 +4605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="n">
         <v>27278725</v>
       </c>
@@ -4441,7 +4625,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="n">
         <v>27278725</v>
       </c>
@@ -4461,7 +4645,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="n">
         <v>27278725</v>
       </c>
@@ -4481,7 +4665,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="n">
         <v>27278725</v>
       </c>
@@ -4501,7 +4685,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="n">
         <v>27278725</v>
       </c>
@@ -4521,7 +4705,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="n">
         <v>27278725</v>
       </c>
@@ -4541,7 +4725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="n">
         <v>27341108</v>
       </c>
@@ -4561,7 +4745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="n">
         <v>27341108</v>
       </c>
@@ -4581,7 +4765,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="n">
         <v>27341108</v>
       </c>
@@ -4601,7 +4785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="n">
         <v>27341108</v>
       </c>
@@ -4621,7 +4805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="n">
         <v>27341108</v>
       </c>
@@ -4641,7 +4825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="n">
         <v>27341108</v>
       </c>
@@ -4661,7 +4845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="n">
         <v>27341108</v>
       </c>
@@ -4681,7 +4865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="n">
         <v>27341108</v>
       </c>
@@ -4701,7 +4885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="n">
         <v>27341108</v>
       </c>
@@ -4721,7 +4905,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="n">
         <v>27404981</v>
       </c>
@@ -4741,7 +4925,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="n">
         <v>27404981</v>
       </c>
@@ -4761,7 +4945,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="n">
         <v>27404981</v>
       </c>
@@ -4781,7 +4965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="n">
         <v>27404981</v>
       </c>
@@ -4801,7 +4985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="n">
         <v>27404981</v>
       </c>
@@ -4821,7 +5005,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="n">
         <v>27404981</v>
       </c>
@@ -4841,7 +5025,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="n">
         <v>27528385</v>
       </c>
@@ -4861,7 +5045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="n">
         <v>27528385</v>
       </c>
@@ -4881,7 +5065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="n">
         <v>27974196</v>
       </c>
@@ -4901,7 +5085,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="n">
         <v>27974196</v>
       </c>
@@ -4921,7 +5105,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="n">
         <v>27974196</v>
       </c>
@@ -4941,7 +5125,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="n">
         <v>27974196</v>
       </c>
@@ -4961,7 +5145,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="n">
         <v>27974196</v>
       </c>
@@ -4981,7 +5165,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="n">
         <v>27974196</v>
       </c>
@@ -5001,7 +5185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="n">
         <v>27974196</v>
       </c>
@@ -5021,7 +5205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="n">
         <v>27974196</v>
       </c>
@@ -5041,7 +5225,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="n">
         <v>27974196</v>
       </c>
@@ -5061,7 +5245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="n">
         <v>27974196</v>
       </c>
@@ -5081,7 +5265,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="n">
         <v>27974196</v>
       </c>
@@ -5101,7 +5285,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5121,7 +5305,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5141,7 +5325,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5161,7 +5345,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5181,7 +5365,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5201,7 +5385,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5221,7 +5405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5241,7 +5425,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5261,7 +5445,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5281,7 +5465,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5301,7 +5485,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5321,7 +5505,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5341,7 +5525,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5361,7 +5545,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5381,7 +5565,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5401,7 +5585,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5421,7 +5605,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="n">
         <v>28176813</v>
       </c>
@@ -5439,6 +5623,386 @@
       </c>
       <c r="F211" s="0" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="2" t="n">
+        <v>26035832</v>
+      </c>
+      <c r="B212" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="C212" s="0" t="n">
+        <v>466</v>
+      </c>
+      <c r="D212" s="0" t="n">
+        <v>484</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="F212" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="2" t="n">
+        <v>26035832</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C213" s="0" t="n">
+        <v>464</v>
+      </c>
+      <c r="D213" s="0" t="n">
+        <v>445</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="F213" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="2" t="n">
+        <v>28729655</v>
+      </c>
+      <c r="B214" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="C214" s="0" t="n">
+        <v>272</v>
+      </c>
+      <c r="D214" s="0" t="n">
+        <v>291</v>
+      </c>
+      <c r="E214" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F214" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="2" t="n">
+        <v>28729655</v>
+      </c>
+      <c r="B215" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C215" s="0" t="n">
+        <v>8964</v>
+      </c>
+      <c r="D215" s="0" t="n">
+        <v>8983</v>
+      </c>
+      <c r="E215" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="F215" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="2" t="n">
+        <v>28729655</v>
+      </c>
+      <c r="B216" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="C216" s="0" t="n">
+        <v>8379</v>
+      </c>
+      <c r="D216" s="0" t="n">
+        <v>8398</v>
+      </c>
+      <c r="E216" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="F216" s="0" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="2" t="n">
+        <v>28729655</v>
+      </c>
+      <c r="B217" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C217" s="0" t="n">
+        <v>2982</v>
+      </c>
+      <c r="D217" s="0" t="n">
+        <v>3001</v>
+      </c>
+      <c r="E217" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="F217" s="0" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="n">
+        <v>28670581</v>
+      </c>
+      <c r="B218" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C218" s="0" t="n">
+        <v>465</v>
+      </c>
+      <c r="D218" s="0" t="n">
+        <v>484</v>
+      </c>
+      <c r="E218" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F218" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="n">
+        <v>28670581</v>
+      </c>
+      <c r="B219" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C219" s="0" t="n">
+        <v>343</v>
+      </c>
+      <c r="D219" s="0" t="n">
+        <v>362</v>
+      </c>
+      <c r="E219" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F219" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="2" t="n">
+        <v>28366764</v>
+      </c>
+      <c r="B220" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C220" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="D220" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="E220" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="F220" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="2" t="n">
+        <v>28366764</v>
+      </c>
+      <c r="B221" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C221" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="D221" s="0" t="n">
+        <v>223</v>
+      </c>
+      <c r="E221" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="F221" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="2" t="n">
+        <v>28366764</v>
+      </c>
+      <c r="B222" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C222" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="D222" s="0" t="n">
+        <v>399</v>
+      </c>
+      <c r="E222" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F222" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="2" t="n">
+        <v>28366764</v>
+      </c>
+      <c r="B223" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C223" s="0" t="n">
+        <v>2103</v>
+      </c>
+      <c r="D223" s="0" t="n">
+        <v>2124</v>
+      </c>
+      <c r="E223" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="F223" s="0" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="2" t="n">
+        <v>28366764</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="C224" s="0" t="n">
+        <v>796</v>
+      </c>
+      <c r="D224" s="0" t="n">
+        <v>817</v>
+      </c>
+      <c r="E224" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="F224" s="0" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="2" t="n">
+        <v>28366764</v>
+      </c>
+      <c r="B225" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="C225" s="0" t="n">
+        <v>1061</v>
+      </c>
+      <c r="D225" s="0" t="n">
+        <v>1081</v>
+      </c>
+      <c r="E225" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="F225" s="0" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="2" t="n">
+        <v>28366764</v>
+      </c>
+      <c r="B226" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C226" s="0" t="n">
+        <v>4149</v>
+      </c>
+      <c r="D226" s="0" t="n">
+        <v>4168</v>
+      </c>
+      <c r="E226" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F226" s="0" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="n">
+        <v>25781496</v>
+      </c>
+      <c r="B227" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C227" s="0" t="n">
+        <v>465</v>
+      </c>
+      <c r="D227" s="0" t="n">
+        <v>484</v>
+      </c>
+      <c r="E227" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F227" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="n">
+        <v>27698388</v>
+      </c>
+      <c r="B228" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="C228" s="0" t="n">
+        <v>344</v>
+      </c>
+      <c r="D228" s="0" t="n">
+        <v>363</v>
+      </c>
+      <c r="E228" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="F228" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="n">
+        <v>27698388</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="C229" s="0" t="n">
+        <v>385</v>
+      </c>
+      <c r="D229" s="0" t="n">
+        <v>404</v>
+      </c>
+      <c r="E229" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="F229" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="n">
+        <v>27698388</v>
+      </c>
+      <c r="B230" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="C230" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="D230" s="0" t="n">
+        <v>399</v>
+      </c>
+      <c r="E230" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F230" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>